<commit_message>
Add units for map layers
</commit_message>
<xml_diff>
--- a/src/assets/morvel_velocity.xlsx
+++ b/src/assets/morvel_velocity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuyang/Desktop/InVEST_database/datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lance\Documents\GitHub\Map\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D342B077-80B7-4745-8BAC-9D429F0C5C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6888A2E6-3AB9-4B3B-AB0D-E829209F164A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{B8D10408-699D-7D43-9888-B64CA8745454}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{B8D10408-699D-7D43-9888-B64CA8745454}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,25 +56,25 @@
     <t>EU-SU</t>
   </si>
   <si>
-    <t>Latitude</t>
-  </si>
-  <si>
-    <t>Longitude</t>
-  </si>
-  <si>
-    <t>Velocity (mm/yr)</t>
-  </si>
-  <si>
-    <t>Direction</t>
-  </si>
-  <si>
-    <t>Northward Velocity</t>
-  </si>
-  <si>
-    <t>Eastward velocity</t>
-  </si>
-  <si>
     <t>YZ-SU</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>velocity</t>
+  </si>
+  <si>
+    <t>direction</t>
+  </si>
+  <si>
+    <t>northwardVelocity</t>
+  </si>
+  <si>
+    <t>eastwardVelocity</t>
   </si>
 </sst>
 </file>
@@ -456,38 +456,38 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>20</v>
       </c>
@@ -510,7 +510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>18</v>
       </c>
@@ -533,7 +533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>14</v>
       </c>
@@ -556,7 +556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>11</v>
       </c>
@@ -579,7 +579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>8</v>
       </c>
@@ -602,7 +602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -625,7 +625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>21</v>
       </c>
@@ -648,7 +648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>22</v>
       </c>
@@ -671,7 +671,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>24</v>
       </c>
@@ -694,7 +694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>26.5</v>
       </c>
@@ -717,7 +717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>21</v>
       </c>
@@ -740,7 +740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>19</v>
       </c>
@@ -763,7 +763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>16.600000000000001</v>
       </c>
@@ -786,7 +786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>15</v>
       </c>
@@ -809,7 +809,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>11.5</v>
       </c>
@@ -832,7 +832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>7.3</v>
       </c>
@@ -855,7 +855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>3.3</v>
       </c>
@@ -878,7 +878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>-0.6</v>
       </c>
@@ -901,7 +901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>-4</v>
       </c>
@@ -924,7 +924,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>-8</v>
       </c>
@@ -947,7 +947,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>-11</v>
       </c>
@@ -970,7 +970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>-12</v>
       </c>
@@ -993,7 +993,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>-13</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>-12.5</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>-10</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>16</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>17</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>18.5</v>
       </c>
@@ -1128,10 +1128,10 @@
         <v>0.84</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>16.5</v>
       </c>
@@ -1151,10 +1151,11 @@
         <v>0.63</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>